<commit_message>
Jakieś coś nie wiem co
</commit_message>
<xml_diff>
--- a/testGenerator/test/bin/Debug/zestawPytań2.xlsx
+++ b/testGenerator/test/bin/Debug/zestawPytań2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A034FE9-FE10-44C4-8558-FE14F199AE70}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD25190-0C80-455F-A167-FBD7D3657E32}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,17 +467,16 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="3.5703125" style="2" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>

</xml_diff>